<commit_message>
save 09 12 2025
</commit_message>
<xml_diff>
--- a/4 четверть_4_JavaScript_Back.xlsx
+++ b/4 четверть_4_JavaScript_Back.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D623FEB1-8BA4-461F-9FC1-60088C2AC4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB87AD1-B629-4F94-851D-62B7DC183306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Крутой онлайн debugger" sheetId="1" r:id="rId1"/>
@@ -23479,11 +23479,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -24148,9 +24156,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -24170,164 +24178,164 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="49" fontId="24" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="25" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="10" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -24336,149 +24344,152 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="39" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="41" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="42" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="42" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="38" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="17" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="16" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="17" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -24489,31 +24500,28 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="44" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="43" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="18" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -24522,19 +24530,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -24542,9 +24553,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -26145,9 +26153,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3802527</xdr:colOff>
+      <xdr:colOff>3793002</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1567815</xdr:rowOff>
+      <xdr:rowOff>1577340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -26608,10 +26616,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="128"/>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="A1" s="129"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -27154,7 +27162,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>79</v>
       </c>
@@ -30140,12 +30148,12 @@
       </c>
     </row>
     <row r="316" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A316" s="129" t="s">
+      <c r="A316" s="130" t="s">
         <v>774</v>
       </c>
-      <c r="B316" s="129"/>
-      <c r="C316" s="129"/>
-      <c r="D316" s="129"/>
+      <c r="B316" s="130"/>
+      <c r="C316" s="130"/>
+      <c r="D316" s="130"/>
     </row>
     <row r="317" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A317" s="13"/>
@@ -31451,10 +31459,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="128"/>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
+      <c r="A1" s="129"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -31761,7 +31769,7 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -31797,10 +31805,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="130"/>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
+      <c r="A1" s="131"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -31927,7 +31935,7 @@
       <c r="A13" s="1" t="s">
         <v>934</v>
       </c>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="128" t="s">
         <v>936</v>
       </c>
     </row>
@@ -32224,12 +32232,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>759</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>

</xml_diff>